<commit_message>
Changes in the dictionary and previsualization in a jupyter notebook
</commit_message>
<xml_diff>
--- a/dictionary.xlsx
+++ b/dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Desktop\TwiterDataPresidentElections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DAA3093-F28E-4E98-82DB-4778952E9DD5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C287B1EA-6A9C-44EB-8F0C-05F014CE5489}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4BF6F5E9-DFBE-4611-B447-23387757ACF4}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4BF6F5E9-DFBE-4611-B447-23387757ACF4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -111,9 +111,6 @@
     <t>El número de seguidores que tiene esta cuenta actualmente. Bajo ciertas condiciones de coacción, este campo indicará temporalmente "0"</t>
   </si>
   <si>
-    <t>El número de usuarios que sigue esta cuenta (también conocido como sus "seguidores"). Bajo ciertas condiciones de coacción, este campo indicará temporalmente "0".</t>
-  </si>
-  <si>
     <t>Muestra el lenguaje que el usuario ha registrado en la plataform. Este campo podria ser nulo</t>
   </si>
   <si>
@@ -136,13 +133,39 @@
   </si>
   <si>
     <t>Columna1</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">El número de usuarios que esta cuenta </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF202124"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>esta siguiendo</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF202124"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (también conocido como sus "seguidores"). Bajo ciertas condiciones de coacción, este campo indicará temporalmente "0".</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,6 +205,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -289,6 +320,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF494747"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -300,24 +349,6 @@
         <vertAlign val="baseline"/>
         <sz val="12"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF494747"/>
         <name val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -337,11 +368,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09B487D9-8A78-41F8-80F2-F51FA9F3020D}" name="Tabla1" displayName="Tabla1" ref="A1:D16" totalsRowShown="0" headerRowDxfId="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09B487D9-8A78-41F8-80F2-F51FA9F3020D}" name="Tabla1" displayName="Tabla1" ref="A1:D16" totalsRowShown="0" headerRowDxfId="3">
   <autoFilter ref="A1:D16" xr:uid="{2BCF4044-9D6B-4522-9DA2-D28E573C4005}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{3AE8F108-5C4B-43C7-A69E-6593AD376A8E}" name="Columna1"/>
-    <tableColumn id="2" xr3:uid="{B182A232-30CE-4267-B2D7-29685D4EA894}" name="Campos del Dataset" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{B182A232-30CE-4267-B2D7-29685D4EA894}" name="Campos del Dataset" dataDxfId="2"/>
     <tableColumn id="3" xr3:uid="{B048A49B-8B9B-42F8-8C4E-7CD3545EB6EF}" name="Tipo de Dato" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{B6028168-785D-4B5A-8AFB-34F7A67F8F96}" name="Descripción" dataDxfId="0"/>
   </tableColumns>
@@ -648,8 +679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDE3F67-3D24-4708-959B-DDD357F87E6A}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,7 +692,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>15</v>
@@ -754,7 +785,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -768,7 +799,7 @@
         <v>22</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -824,7 +855,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -838,7 +869,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
@@ -852,7 +883,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="48" thickBot="1" x14ac:dyDescent="0.3">
@@ -866,7 +897,7 @@
         <v>22</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="32.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -877,10 +908,10 @@
         <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>